<commit_message>
finsihed real estate scraping bot
</commit_message>
<xml_diff>
--- a/realestatedata.xlsx
+++ b/realestatedata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ajeffers\Documents\UiPath\UdemyCourse\Robots\Robot4_RealEstateScraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E130BB2-0601-45C6-97C3-991BAB91130E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8566345A-B693-4B9A-A169-D1CCE5D8D22F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="50265" yWindow="2820" windowWidth="13245" windowHeight="7410" xr2:uid="{9CD18BFF-5186-4E85-A5D9-24B5FB4A3B85}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>89 m²</t>
   </si>
@@ -131,9 +131,6 @@
     <t>Tokai</t>
   </si>
   <si>
-    <t>R 3 299 000</t>
-  </si>
-  <si>
     <t>81 m²</t>
   </si>
   <si>
@@ -194,10 +191,7 @@
     <t>R 999 999</t>
   </si>
   <si>
-    <t>R 1 995 000</t>
-  </si>
-  <si>
-    <t>109 m²</t>
+    <t>R 3 300 000</t>
   </si>
 </sst>
 </file>
@@ -670,7 +664,7 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D7" t="s">
         <v>22</v>
@@ -698,19 +692,19 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>3</v>
       </c>
       <c r="C9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
@@ -749,7 +743,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -758,27 +752,27 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
         <v>33</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
         <v>33</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.45">
@@ -792,117 +786,117 @@
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B17">
         <v>3</v>
       </c>
       <c r="C17">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
       <c r="C19">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="D20" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21">
         <v>2</v>
@@ -919,7 +913,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22">
         <v>2</v>

</xml_diff>